<commit_message>
Updates to aspen fires plot
</commit_message>
<xml_diff>
--- a/Aim3/figures/variable_table.xlsx
+++ b/Aim3/figures/variable_table.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim3/data/tabular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim3/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="419" documentId="8_{C9994871-72E6-B147-955B-36EC901D5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62891448-B804-7B4C-8358-DFE7FA7A00D8}"/>
+  <xr:revisionPtr revIDLastSave="428" documentId="8_{C9994871-72E6-B147-955B-36EC901D5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93477506-772D-A546-85EF-11E24582994B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E25C0F8B-5D1F-D74F-95BE-F0194400311A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="version 02" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
   <si>
     <t>Category</t>
   </si>
@@ -321,6 +322,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2041-2070 Aspen suitability change (SSP585) </t>
   </si>
 </sst>
 </file>
@@ -427,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -478,9 +482,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,7 +825,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1181,7 @@
     </row>
     <row r="18" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
-      <c r="B18" s="18"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
@@ -1320,4 +1321,449 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B5033B-EF70-F742-A412-F7FC89E39798}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final "" updates to SOM analysis and figures
</commit_message>
<xml_diff>
--- a/Aim3/figures/variable_table.xlsx
+++ b/Aim3/figures/variable_table.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim3/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="428" documentId="8_{C9994871-72E6-B147-955B-36EC901D5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93477506-772D-A546-85EF-11E24582994B}"/>
+  <xr:revisionPtr revIDLastSave="594" documentId="8_{C9994871-72E6-B147-955B-36EC901D5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F91AEAC-3BFB-D740-A24C-06DFE1FC6EA9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E25C0F8B-5D1F-D74F-95BE-F0194400311A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{E25C0F8B-5D1F-D74F-95BE-F0194400311A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="version 02" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="125">
   <si>
     <t>Category</t>
   </si>
@@ -324,7 +324,142 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">2041-2070 Aspen suitability change (SSP585) </t>
+    <t>Aspen</t>
+  </si>
+  <si>
+    <t>Contemporary aspen canopy cover (hectares)</t>
+  </si>
+  <si>
+    <t>aspen_ha</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>Aggregation method</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Average patch size</t>
+  </si>
+  <si>
+    <t>patch_size</t>
+  </si>
+  <si>
+    <t>Cook et al., 2025</t>
+  </si>
+  <si>
+    <t>Patch density</t>
+  </si>
+  <si>
+    <t>patch_den</t>
+  </si>
+  <si>
+    <t>big_patch</t>
+  </si>
+  <si>
+    <t>Cook et al., 2026</t>
+  </si>
+  <si>
+    <t>Cook et al., 2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in aspen habitat suitability  (SSP585; 2041-2070) </t>
+  </si>
+  <si>
+    <t>burned_pct</t>
+  </si>
+  <si>
+    <t>disturbed</t>
+  </si>
+  <si>
+    <t>Disturbance (%)</t>
+  </si>
+  <si>
+    <t>Firesheds</t>
+  </si>
+  <si>
+    <t>pop_den</t>
+  </si>
+  <si>
+    <t>Population density</t>
+  </si>
+  <si>
+    <t>WUI (%)</t>
+  </si>
+  <si>
+    <t>Forest characteristic</t>
+  </si>
+  <si>
+    <t>lf_canopy</t>
+  </si>
+  <si>
+    <t>lf_height</t>
+  </si>
+  <si>
+    <t>Forested percent</t>
+  </si>
+  <si>
+    <t>forest_pct</t>
+  </si>
+  <si>
+    <t>Conditional flame length</t>
+  </si>
+  <si>
+    <t>cfl_p90</t>
+  </si>
+  <si>
+    <t>90th percentile</t>
+  </si>
+  <si>
+    <t>LANDFIRE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Uhl et al., </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Schoolbook"/>
+        <family val="1"/>
+      </rPr>
+      <t>In prep</t>
+    </r>
+  </si>
+  <si>
+    <t>Historic &amp; future fire activity / disturbance</t>
+  </si>
+  <si>
+    <t>Distance to WUI</t>
+  </si>
+  <si>
+    <t>wui_dist</t>
+  </si>
+  <si>
+    <t>Housing unit impact</t>
+  </si>
+  <si>
+    <t>hui_p90</t>
+  </si>
+  <si>
+    <t>Wildfire hazard  potential</t>
+  </si>
+  <si>
+    <t>whp_p90</t>
+  </si>
+  <si>
+    <t>Wildfire exposure</t>
+  </si>
+  <si>
+    <t>exposure</t>
+  </si>
+  <si>
+    <t>Fire hazard / vulnerability</t>
   </si>
 </sst>
 </file>
@@ -374,7 +509,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -427,11 +562,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -482,6 +646,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3CA0B3-B9A1-D745-AA65-486A423CA385}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1325,445 +1510,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B5033B-EF70-F742-A412-F7FC89E39798}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>41</v>
+        <v>83</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E6" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5" t="s">
+    <row r="7" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="E7" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E9" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E10" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7" t="s">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E17" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E21" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
+  <mergeCells count="4">
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>